<commit_message>
Add more tests. Fix bug in get pictures map.
</commit_message>
<xml_diff>
--- a/tests/resources/sheet/datacommentdemo.xlsx
+++ b/tests/resources/sheet/datacommentdemo.xlsx
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Department:</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>${employee.sex}</t>
+  </si>
+  <si>
+    <t>Test area formula</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -719,6 +722,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -764,7 +778,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -820,6 +834,9 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -834,6 +851,9 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -888,6 +908,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>608700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2354580" y="91440"/>
+          <a:ext cx="1775460" cy="517260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1177,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1191,63 +1260,68 @@
     <col min="4" max="4" width="14.36328125" customWidth="1"/>
     <col min="5" max="6" width="11.36328125" customWidth="1"/>
     <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
-    <row r="3" spans="1:7" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="1:7" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="22">
         <f>COUNT((G8))</f>
         <v>0</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:7" ht="37.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="37.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1256,7 +1330,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -1278,8 +1352,11 @@
       <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="H7" s="19" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -1302,8 +1379,12 @@
         <f>E8*(1+F8)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H8">
+        <f>SUM((E8:F8))</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1319,8 +1400,12 @@
         <f>SUM((G8))</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H9">
+        <f>SUM((E8:F8))</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1328,16 +1413,22 @@
         <f>SUM((G9))</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H10">
+        <f>SUM((E8:F8))</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.69861111111111107" right="0.69861111111111107" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>